<commit_message>
primeira aula sobre simplex
</commit_message>
<xml_diff>
--- a/PesquisaOperacional/2/aula0503/SimplexExemplo01.xlsx
+++ b/PesquisaOperacional/2/aula0503/SimplexExemplo01.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
   <si>
     <t>coeficiente</t>
   </si>
   <si>
-    <t>variável básica</t>
-  </si>
-  <si>
     <t>nº</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>x5</t>
   </si>
   <si>
-    <t>lado direito</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -63,14 +57,45 @@
   </si>
   <si>
     <t>1/2</t>
+  </si>
+  <si>
+    <t>variável</t>
+  </si>
+  <si>
+    <t>direita</t>
+  </si>
+  <si>
+    <t>3/2</t>
+  </si>
+  <si>
+    <t>1/3</t>
+  </si>
+  <si>
+    <t>-1/3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -180,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,6 +220,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -207,16 +244,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -499,70 +531,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:I13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="12" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="A1" s="8">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -570,7 +597,7 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="6">
         <v>-3</v>
       </c>
       <c r="E3" s="5">
@@ -591,7 +618,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -619,8 +646,8 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
+      <c r="A5" s="14" t="s">
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -631,7 +658,7 @@
       <c r="D5" s="5">
         <v>0</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="7">
         <v>2</v>
       </c>
       <c r="F5" s="5">
@@ -651,7 +678,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
@@ -680,63 +707,63 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -744,20 +771,20 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <v>-3</v>
       </c>
       <c r="E10" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>11</v>
+      <c r="G10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
       </c>
       <c r="I10" s="3">
         <v>30</v>
@@ -765,7 +792,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -794,7 +821,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -811,8 +838,8 @@
       <c r="F12" s="5">
         <v>0</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>12</v>
+      <c r="G12" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H12" s="5">
         <v>0</v>
@@ -822,8 +849,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
+      <c r="A13" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -850,11 +877,176 @@
         <v>6</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B15:I15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>